<commit_message>
Preparations for hysteresis test
</commit_message>
<xml_diff>
--- a/RPMvsPWM-1.xlsx
+++ b/RPMvsPWM-1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>NOTE :</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Higher frequency (kept in limit of Motor driver i.e. 3kHz in our case) linearizes the PWM vs RPM plot but at lower duty cycle for high frequency it affects torque of motor and also can lead heating of motor and motor driver</t>
+  </si>
+  <si>
+    <t>NOTE : Divide all the  frequencies in legend by 64 for actual frequency. Clock divisor of 64 factor was implemented when these readings were taken which was overlooked</t>
   </si>
 </sst>
 </file>
@@ -102,12 +105,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,17 +131,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -529,15 +541,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="Q81" sqref="Q81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -545,13 +557,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+    </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -575,8 +616,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -998,7 +1039,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -1011,7 +1052,7 @@
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
-      <c r="K56" s="4"/>
+      <c r="K56" s="2"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C57" s="5"/>
@@ -1034,10 +1075,11 @@
       <c r="J58" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A39:XFD39"/>
     <mergeCell ref="C56:J58"/>
+    <mergeCell ref="N13:T15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>